<commit_message>
Recoded NA as missing in quality assessment questions
</commit_message>
<xml_diff>
--- a/input/20211201-study.characteristics_update.xlsx
+++ b/input/20211201-study.characteristics_update.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\SR_prevalence_NTM\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCFEB563-3A83-49AB-9BDF-9FC30D5CADB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE89B2E5-C0AC-462F-A9F3-AE8E7780F653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="600" windowWidth="4950" windowHeight="10920" xr2:uid="{9BAFF895-4EE1-48C5-B0C9-C001584A386E}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" xr2:uid="{9BAFF895-4EE1-48C5-B0C9-C001584A386E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -3254,9 +3254,6 @@
     <t xml:space="preserve">Scandinavian CF populatoion </t>
   </si>
   <si>
-    <t>Correction: 4/130 (3.08)</t>
-  </si>
-  <si>
     <t>Smith1984</t>
   </si>
   <si>
@@ -21131,6 +21128,9 @@
 11.6 (7.4–15.9)
 [median;range]</t>
     </r>
+  </si>
+  <si>
+    <t>4/130 (3.08)</t>
   </si>
 </sst>
 </file>
@@ -21265,7 +21265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -21332,22 +21332,11 @@
     <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0070C0"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF0070C0"/>
@@ -21691,9 +21680,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AQ96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH99" sqref="AH99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15"/>
@@ -21741,7 +21730,7 @@
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
@@ -21870,12 +21859,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:43" ht="158.25" customHeight="1">
+    <row r="2" spans="1:43" ht="158.25" hidden="1" customHeight="1">
       <c r="A2" s="6" t="s">
+        <v>939</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>940</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>941</v>
       </c>
       <c r="C2" s="7">
         <v>2021</v>
@@ -21884,13 +21873,13 @@
         <v>204</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F2" s="7">
         <v>485</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>31</v>
@@ -21899,34 +21888,34 @@
         <v>67</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>161</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="7" t="s">
+        <v>1013</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>1014</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>1015</v>
       </c>
-      <c r="P2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>942</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>1016</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>943</v>
       </c>
       <c r="T2" s="7" t="s">
         <v>268</v>
@@ -21947,38 +21936,38 @@
         <v>46</v>
       </c>
       <c r="Z2" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="AA2" s="7" t="s">
         <v>944</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AB2" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="AD2" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="AE2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH2" s="9" t="s">
         <v>945</v>
       </c>
-      <c r="AB2" s="8" t="s">
-        <v>955</v>
-      </c>
-      <c r="AC2" s="8" t="s">
-        <v>954</v>
-      </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AI2" s="9" t="s">
+        <v>983</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
         <v>947</v>
       </c>
-      <c r="AE2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH2" s="9" t="s">
-        <v>946</v>
-      </c>
-      <c r="AI2" s="9" t="s">
-        <v>984</v>
-      </c>
-      <c r="AJ2" s="7" t="s">
-        <v>948</v>
-      </c>
       <c r="AK2" s="7" t="s">
         <v>46</v>
       </c>
@@ -21989,24 +21978,24 @@
         <v>46</v>
       </c>
       <c r="AN2" s="7" t="s">
+        <v>1016</v>
+      </c>
+      <c r="AO2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP2" s="7" t="s">
         <v>1017</v>
-      </c>
-      <c r="AO2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP2" s="7" t="s">
-        <v>1018</v>
       </c>
       <c r="AQ2" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:43" ht="240">
+    <row r="3" spans="1:43" ht="225" hidden="1">
       <c r="A3" s="5" t="s">
+        <v>959</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>960</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>961</v>
       </c>
       <c r="C3" s="7">
         <v>2021</v>
@@ -22015,16 +22004,16 @@
         <v>48</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F3" s="7">
         <v>171</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>107</v>
@@ -22036,13 +22025,13 @@
         <v>535</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="M3" s="7" t="s">
         <v>102</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="O3" s="10">
         <v>0.54900000000000004</v>
@@ -22051,64 +22040,64 @@
         <v>46</v>
       </c>
       <c r="Q3" s="7" t="s">
+        <v>1019</v>
+      </c>
+      <c r="R3" s="7" t="s">
         <v>1020</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>1021</v>
-      </c>
-      <c r="S3" s="7" t="s">
-        <v>1022</v>
       </c>
       <c r="T3" s="7" t="s">
         <v>268</v>
       </c>
       <c r="U3" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" s="7" t="s">
         <v>964</v>
       </c>
-      <c r="V3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="W3" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>965</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="Y3" s="7" t="s">
         <v>966</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>967</v>
       </c>
       <c r="Z3" s="7" t="s">
         <v>102</v>
       </c>
       <c r="AA3" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="AB3" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="AD3" s="7" t="s">
+        <v>1024</v>
+      </c>
+      <c r="AE3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>993</v>
+      </c>
+      <c r="AI3" s="9" t="s">
+        <v>994</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
         <v>968</v>
-      </c>
-      <c r="AB3" s="7" t="s">
-        <v>1023</v>
-      </c>
-      <c r="AC3" s="7" t="s">
-        <v>1024</v>
-      </c>
-      <c r="AD3" s="7" t="s">
-        <v>1025</v>
-      </c>
-      <c r="AE3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH3" s="9" t="s">
-        <v>994</v>
-      </c>
-      <c r="AI3" s="9" t="s">
-        <v>995</v>
-      </c>
-      <c r="AJ3" s="7" t="s">
-        <v>969</v>
       </c>
       <c r="AK3" s="7" t="s">
         <v>46</v>
@@ -22123,21 +22112,21 @@
         <v>0</v>
       </c>
       <c r="AO3" s="7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="AP3" s="7" t="s">
+        <v>952</v>
+      </c>
+      <c r="AQ3" s="7" t="s">
         <v>1026</v>
       </c>
-      <c r="AP3" s="7" t="s">
-        <v>953</v>
-      </c>
-      <c r="AQ3" s="7" t="s">
-        <v>1027</v>
-      </c>
     </row>
-    <row r="4" spans="1:43" ht="269.25" customHeight="1">
+    <row r="4" spans="1:43" ht="269.25" hidden="1" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C4" s="7">
         <v>2021</v>
@@ -22152,7 +22141,7 @@
         <v>567</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>31</v>
@@ -22161,37 +22150,37 @@
         <v>29</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>535</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="M4" s="7" t="s">
         <v>102</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="O4" s="10" t="s">
+        <v>997</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="Q4" s="7" t="s">
+        <v>1027</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="S4" s="7" t="s">
         <v>998</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>973</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>1028</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>966</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>999</v>
-      </c>
-      <c r="T4" s="7" t="s">
-        <v>974</v>
       </c>
       <c r="U4" s="7" t="s">
         <v>603</v>
@@ -22200,10 +22189,10 @@
         <v>239</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>46</v>
@@ -22212,34 +22201,34 @@
         <v>102</v>
       </c>
       <c r="AA4" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="AB4" s="7" t="s">
         <v>976</v>
       </c>
-      <c r="AB4" s="7" t="s">
+      <c r="AC4" s="7" t="s">
         <v>977</v>
       </c>
-      <c r="AC4" s="7" t="s">
+      <c r="AD4" s="7" t="s">
         <v>978</v>
       </c>
-      <c r="AD4" s="7" t="s">
+      <c r="AE4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AH4" s="9" t="s">
         <v>979</v>
       </c>
-      <c r="AE4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH4" s="9" t="s">
+      <c r="AI4" s="9" t="s">
+        <v>999</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
         <v>980</v>
-      </c>
-      <c r="AI4" s="9" t="s">
-        <v>1000</v>
-      </c>
-      <c r="AJ4" s="7" t="s">
-        <v>981</v>
       </c>
       <c r="AK4" s="7" t="s">
         <v>46</v>
@@ -22254,21 +22243,21 @@
         <v>276</v>
       </c>
       <c r="AO4" s="7" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="AP4" s="7" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AQ4" s="7" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="90">
+    <row r="5" spans="1:43" ht="90" hidden="1">
       <c r="A5" s="5" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C5" s="7">
         <v>2018</v>
@@ -22277,19 +22266,19 @@
         <v>48</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F5" s="7">
         <v>124</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>31</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>462</v>
@@ -22298,13 +22287,13 @@
         <v>535</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>102</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="O5" s="10">
         <v>0.47</v>
@@ -22322,7 +22311,7 @@
         <v>46</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="U5" s="7" t="s">
         <v>603</v>
@@ -22331,7 +22320,7 @@
         <v>46</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="X5" s="7" t="s">
         <v>490</v>
@@ -22340,19 +22329,19 @@
         <v>46</v>
       </c>
       <c r="Z5" s="7" t="s">
+        <v>989</v>
+      </c>
+      <c r="AA5" s="7" t="s">
+        <v>1028</v>
+      </c>
+      <c r="AB5" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="AC5" s="8" t="s">
+        <v>956</v>
+      </c>
+      <c r="AD5" s="7" t="s">
         <v>990</v>
-      </c>
-      <c r="AA5" s="7" t="s">
-        <v>1029</v>
-      </c>
-      <c r="AB5" s="7" t="s">
-        <v>956</v>
-      </c>
-      <c r="AC5" s="8" t="s">
-        <v>957</v>
-      </c>
-      <c r="AD5" s="7" t="s">
-        <v>991</v>
       </c>
       <c r="AE5" s="7" t="s">
         <v>46</v>
@@ -22364,13 +22353,13 @@
         <v>46</v>
       </c>
       <c r="AH5" s="9" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="AI5" s="9" t="s">
         <v>46</v>
       </c>
       <c r="AJ5" s="7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="AK5" s="7" t="s">
         <v>46</v>
@@ -22388,7 +22377,7 @@
         <v>276</v>
       </c>
       <c r="AP5" s="7" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="AQ5" s="7" t="s">
         <v>276</v>
@@ -22396,7 +22385,7 @@
     </row>
     <row r="6" spans="1:43" ht="150" hidden="1">
       <c r="A6" s="1" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>134</v>
@@ -22435,22 +22424,22 @@
         <v>140</v>
       </c>
       <c r="N6" s="7" t="s">
+        <v>1029</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>1030</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>1031</v>
       </c>
-      <c r="P6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q6" s="7" t="s">
+      <c r="R6" s="7" t="s">
         <v>1032</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>1033</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>1034</v>
       </c>
       <c r="T6" s="7" t="s">
         <v>71</v>
@@ -22519,7 +22508,7 @@
         <v>46</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="AQ6" s="7" t="s">
         <v>46</v>
@@ -22527,7 +22516,7 @@
     </row>
     <row r="7" spans="1:43" ht="60" hidden="1">
       <c r="A7" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>145</v>
@@ -22658,7 +22647,7 @@
     </row>
     <row r="8" spans="1:43" ht="240" hidden="1">
       <c r="A8" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>158</v>
@@ -22697,22 +22686,22 @@
         <v>151</v>
       </c>
       <c r="N8" s="7" t="s">
+        <v>1035</v>
+      </c>
+      <c r="O8" s="7" t="s">
         <v>1036</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R8" s="7" t="s">
         <v>1037</v>
       </c>
-      <c r="P8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R8" s="7" t="s">
+      <c r="S8" s="7" t="s">
         <v>1038</v>
-      </c>
-      <c r="S8" s="7" t="s">
-        <v>1039</v>
       </c>
       <c r="T8" s="7" t="s">
         <v>163</v>
@@ -22757,7 +22746,7 @@
         <v>164</v>
       </c>
       <c r="AH8" s="9" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="AI8" s="9" t="s">
         <v>46</v>
@@ -22778,18 +22767,18 @@
         <v>46</v>
       </c>
       <c r="AO8" s="7" t="s">
+        <v>1040</v>
+      </c>
+      <c r="AP8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ8" s="7" t="s">
         <v>1041</v>
-      </c>
-      <c r="AP8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ8" s="7" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="9" spans="1:43" ht="90" hidden="1">
       <c r="A9" s="1" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>23</v>
@@ -22920,7 +22909,7 @@
     </row>
     <row r="10" spans="1:43" ht="105" hidden="1">
       <c r="A10" s="4" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>118</v>
@@ -22959,22 +22948,22 @@
         <v>46</v>
       </c>
       <c r="N10" s="7" t="s">
+        <v>1042</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>1043</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="P10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q10" s="7" t="s">
         <v>1044</v>
       </c>
-      <c r="P10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q10" s="7" t="s">
+      <c r="R10" s="7" t="s">
         <v>1045</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="S10" s="7" t="s">
         <v>1046</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>1047</v>
       </c>
       <c r="T10" s="7" t="s">
         <v>125</v>
@@ -23051,7 +23040,7 @@
     </row>
     <row r="11" spans="1:43" ht="150" hidden="1">
       <c r="A11" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>195</v>
@@ -23066,7 +23055,7 @@
         <v>95</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>196</v>
@@ -23090,16 +23079,16 @@
         <v>46</v>
       </c>
       <c r="N11" s="7" t="s">
+        <v>1048</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>1049</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="P11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="7" t="s">
         <v>1050</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" s="7" t="s">
-        <v>1051</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>46</v>
@@ -23182,7 +23171,7 @@
     </row>
     <row r="12" spans="1:43" ht="150" hidden="1">
       <c r="A12" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>606</v>
@@ -23224,16 +23213,16 @@
         <v>612</v>
       </c>
       <c r="O12" s="7" t="s">
+        <v>1051</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" s="7" t="s">
         <v>1052</v>
       </c>
-      <c r="P12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q12" s="7" t="s">
+      <c r="R12" s="7" t="s">
         <v>1053</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>1054</v>
       </c>
       <c r="S12" s="7" t="s">
         <v>46</v>
@@ -23299,7 +23288,7 @@
         <v>46</v>
       </c>
       <c r="AN12" s="7" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="AO12" s="7" t="s">
         <v>613</v>
@@ -23308,12 +23297,12 @@
         <v>46</v>
       </c>
       <c r="AQ12" s="7" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="13" spans="1:43" ht="165" hidden="1">
       <c r="A13" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>615</v>
@@ -23352,19 +23341,19 @@
         <v>618</v>
       </c>
       <c r="N13" s="7" t="s">
+        <v>1056</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>1057</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="P13" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q13" s="7" t="s">
         <v>1058</v>
       </c>
-      <c r="P13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q13" s="7" t="s">
+      <c r="R13" s="7" t="s">
         <v>1059</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>1060</v>
       </c>
       <c r="S13" s="7" t="s">
         <v>46</v>
@@ -23430,7 +23419,7 @@
         <v>46</v>
       </c>
       <c r="AN13" s="7" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="AO13" s="7" t="s">
         <v>621</v>
@@ -23439,12 +23428,12 @@
         <v>46</v>
       </c>
       <c r="AQ13" s="7" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="180" hidden="1">
       <c r="A14" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>622</v>
@@ -23483,22 +23472,22 @@
         <v>626</v>
       </c>
       <c r="N14" s="7" t="s">
+        <v>1062</v>
+      </c>
+      <c r="O14" s="7" t="s">
         <v>1063</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="P14" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q14" s="7" t="s">
         <v>1064</v>
       </c>
-      <c r="P14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q14" s="7" t="s">
+      <c r="R14" s="7" t="s">
         <v>1065</v>
       </c>
-      <c r="R14" s="7" t="s">
+      <c r="S14" s="7" t="s">
         <v>1066</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>1067</v>
       </c>
       <c r="T14" s="7" t="s">
         <v>276</v>
@@ -23561,7 +23550,7 @@
         <v>46</v>
       </c>
       <c r="AN14" s="7" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="AO14" s="7" t="s">
         <v>628</v>
@@ -23570,12 +23559,12 @@
         <v>46</v>
       </c>
       <c r="AQ14" s="7" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="15" spans="1:43" ht="225" hidden="1">
       <c r="A15" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>629</v>
@@ -23614,22 +23603,22 @@
         <v>632</v>
       </c>
       <c r="N15" s="7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="O15" s="7" t="s">
         <v>1070</v>
       </c>
-      <c r="O15" s="7" t="s">
+      <c r="P15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="7" t="s">
         <v>1071</v>
       </c>
-      <c r="P15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q15" s="7" t="s">
+      <c r="R15" s="7" t="s">
         <v>1072</v>
       </c>
-      <c r="R15" s="7" t="s">
+      <c r="S15" s="7" t="s">
         <v>1073</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>1074</v>
       </c>
       <c r="T15" s="7" t="s">
         <v>276</v>
@@ -23692,7 +23681,7 @@
         <v>46</v>
       </c>
       <c r="AN15" s="7" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="AO15" s="7" t="s">
         <v>634</v>
@@ -23701,12 +23690,12 @@
         <v>46</v>
       </c>
       <c r="AQ15" s="7" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="16" spans="1:43" ht="240" hidden="1">
       <c r="A16" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>635</v>
@@ -23745,22 +23734,22 @@
         <v>637</v>
       </c>
       <c r="N16" s="7" t="s">
+        <v>1076</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>1063</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q16" s="7" t="s">
         <v>1077</v>
       </c>
-      <c r="O16" s="7" t="s">
-        <v>1064</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q16" s="7" t="s">
+      <c r="R16" s="7" t="s">
         <v>1078</v>
       </c>
-      <c r="R16" s="7" t="s">
+      <c r="S16" s="7" t="s">
         <v>1079</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>1080</v>
       </c>
       <c r="T16" s="7" t="s">
         <v>276</v>
@@ -23823,7 +23812,7 @@
         <v>46</v>
       </c>
       <c r="AN16" s="7" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="AO16" s="7" t="s">
         <v>639</v>
@@ -23832,12 +23821,12 @@
         <v>46</v>
       </c>
       <c r="AQ16" s="7" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="17" spans="1:43" ht="240" hidden="1">
       <c r="A17" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>635</v>
@@ -23876,22 +23865,22 @@
         <v>642</v>
       </c>
       <c r="N17" s="7" t="s">
+        <v>1082</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>1063</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q17" s="7" t="s">
         <v>1083</v>
       </c>
-      <c r="O17" s="7" t="s">
-        <v>1064</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q17" s="7" t="s">
+      <c r="R17" s="7" t="s">
         <v>1084</v>
       </c>
-      <c r="R17" s="7" t="s">
+      <c r="S17" s="7" t="s">
         <v>1085</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>1086</v>
       </c>
       <c r="T17" s="7" t="s">
         <v>276</v>
@@ -23954,7 +23943,7 @@
         <v>46</v>
       </c>
       <c r="AN17" s="7" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="AO17" s="7" t="s">
         <v>645</v>
@@ -23963,12 +23952,12 @@
         <v>46</v>
       </c>
       <c r="AQ17" s="7" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="18" spans="1:43" ht="240" hidden="1">
       <c r="A18" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>646</v>
@@ -24007,22 +23996,22 @@
         <v>650</v>
       </c>
       <c r="N18" s="7" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="P18" s="7" t="s">
         <v>46</v>
       </c>
       <c r="Q18" s="7" t="s">
+        <v>1088</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>1078</v>
+      </c>
+      <c r="S18" s="7" t="s">
         <v>1089</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>1079</v>
-      </c>
-      <c r="S18" s="7" t="s">
-        <v>1090</v>
       </c>
       <c r="T18" s="7" t="s">
         <v>276</v>
@@ -24085,7 +24074,7 @@
         <v>46</v>
       </c>
       <c r="AN18" s="7" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="AO18" s="7" t="s">
         <v>652</v>
@@ -24094,12 +24083,12 @@
         <v>46</v>
       </c>
       <c r="AQ18" s="7" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="19" spans="1:43" ht="240" hidden="1">
       <c r="A19" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>653</v>
@@ -24138,22 +24127,22 @@
         <v>656</v>
       </c>
       <c r="N19" s="7" t="s">
+        <v>1092</v>
+      </c>
+      <c r="O19" s="7" t="s">
         <v>1093</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="P19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q19" s="7" t="s">
         <v>1094</v>
       </c>
-      <c r="P19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q19" s="7" t="s">
+      <c r="R19" s="7" t="s">
         <v>1095</v>
       </c>
-      <c r="R19" s="7" t="s">
+      <c r="S19" s="7" t="s">
         <v>1096</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>1097</v>
       </c>
       <c r="T19" s="7" t="s">
         <v>276</v>
@@ -24216,7 +24205,7 @@
         <v>46</v>
       </c>
       <c r="AN19" s="7" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="AO19" s="7" t="s">
         <v>658</v>
@@ -24225,12 +24214,12 @@
         <v>46</v>
       </c>
       <c r="AQ19" s="7" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="20" spans="1:43" ht="60" hidden="1">
       <c r="A20" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>803</v>
@@ -24361,7 +24350,7 @@
     </row>
     <row r="21" spans="1:43" ht="270" hidden="1">
       <c r="A21" s="4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>203</v>
@@ -24400,22 +24389,22 @@
         <v>208</v>
       </c>
       <c r="N21" s="7" t="s">
+        <v>1099</v>
+      </c>
+      <c r="O21" s="7" t="s">
         <v>1100</v>
       </c>
-      <c r="O21" s="7" t="s">
+      <c r="P21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q21" s="7" t="s">
         <v>1101</v>
-      </c>
-      <c r="P21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q21" s="7" t="s">
-        <v>1102</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>216</v>
       </c>
       <c r="S21" s="7" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="T21" s="7" t="s">
         <v>209</v>
@@ -24451,10 +24440,10 @@
         <v>46</v>
       </c>
       <c r="AE21" s="7" t="s">
+        <v>1103</v>
+      </c>
+      <c r="AF21" s="12" t="s">
         <v>1104</v>
-      </c>
-      <c r="AF21" s="12" t="s">
-        <v>1105</v>
       </c>
       <c r="AG21" s="7" t="s">
         <v>218</v>
@@ -24475,16 +24464,16 @@
         <v>46</v>
       </c>
       <c r="AM21" s="7" t="s">
+        <v>1105</v>
+      </c>
+      <c r="AN21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO21" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP21" s="7" t="s">
         <v>1106</v>
-      </c>
-      <c r="AN21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO21" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP21" s="7" t="s">
-        <v>1107</v>
       </c>
       <c r="AQ21" s="7" t="s">
         <v>222</v>
@@ -24492,7 +24481,7 @@
     </row>
     <row r="22" spans="1:43" ht="180" hidden="1">
       <c r="A22" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>223</v>
@@ -24504,7 +24493,7 @@
         <v>204</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="F22" s="7">
         <v>5403</v>
@@ -24531,22 +24520,22 @@
         <v>46</v>
       </c>
       <c r="N22" s="7" t="s">
+        <v>1108</v>
+      </c>
+      <c r="O22" s="7" t="s">
         <v>1109</v>
       </c>
-      <c r="O22" s="7" t="s">
+      <c r="P22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q22" s="7" t="s">
         <v>1110</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q22" s="7" t="s">
-        <v>1111</v>
       </c>
       <c r="R22" s="7" t="s">
         <v>227</v>
       </c>
       <c r="S22" s="7" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>71</v>
@@ -24623,7 +24612,7 @@
     </row>
     <row r="23" spans="1:43" ht="120" hidden="1">
       <c r="A23" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>660</v>
@@ -24668,16 +24657,16 @@
         <v>662</v>
       </c>
       <c r="P23" s="7" t="s">
+        <v>1112</v>
+      </c>
+      <c r="Q23" s="7" t="s">
         <v>1113</v>
       </c>
-      <c r="Q23" s="7" t="s">
+      <c r="R23" s="7" t="s">
         <v>1114</v>
       </c>
-      <c r="R23" s="7" t="s">
+      <c r="S23" s="7" t="s">
         <v>1115</v>
-      </c>
-      <c r="S23" s="7" t="s">
-        <v>1116</v>
       </c>
       <c r="T23" s="7" t="s">
         <v>46</v>
@@ -24740,7 +24729,7 @@
         <v>46</v>
       </c>
       <c r="AN23" s="7" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="AO23" s="7" t="s">
         <v>667</v>
@@ -24749,12 +24738,12 @@
         <v>46</v>
       </c>
       <c r="AQ23" s="7" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="24" spans="1:43" ht="120" hidden="1">
       <c r="A24" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>668</v>
@@ -24793,22 +24782,22 @@
         <v>664</v>
       </c>
       <c r="N24" s="7" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="O24" s="7" t="s">
         <v>669</v>
       </c>
       <c r="P24" s="7" t="s">
+        <v>1119</v>
+      </c>
+      <c r="Q24" s="7" t="s">
         <v>1120</v>
       </c>
-      <c r="Q24" s="7" t="s">
+      <c r="R24" s="7" t="s">
         <v>1121</v>
       </c>
-      <c r="R24" s="7" t="s">
+      <c r="S24" s="7" t="s">
         <v>1122</v>
-      </c>
-      <c r="S24" s="7" t="s">
-        <v>1123</v>
       </c>
       <c r="T24" s="7" t="s">
         <v>46</v>
@@ -24871,21 +24860,21 @@
         <v>46</v>
       </c>
       <c r="AN24" s="7" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="AO24" s="7" t="s">
         <v>671</v>
       </c>
       <c r="AP24" s="7" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="AQ24" s="7" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="25" spans="1:43" ht="165" hidden="1">
       <c r="A25" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>672</v>
@@ -24924,22 +24913,22 @@
         <v>664</v>
       </c>
       <c r="N25" s="7" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="O25" s="7" t="s">
         <v>674</v>
       </c>
       <c r="P25" s="7" t="s">
+        <v>1126</v>
+      </c>
+      <c r="Q25" s="7" t="s">
         <v>1127</v>
       </c>
-      <c r="Q25" s="7" t="s">
+      <c r="R25" s="7" t="s">
         <v>1128</v>
       </c>
-      <c r="R25" s="7" t="s">
+      <c r="S25" s="7" t="s">
         <v>1129</v>
-      </c>
-      <c r="S25" s="7" t="s">
-        <v>1130</v>
       </c>
       <c r="T25" s="7" t="s">
         <v>46</v>
@@ -25002,21 +24991,21 @@
         <v>46</v>
       </c>
       <c r="AN25" s="7" t="s">
+        <v>1130</v>
+      </c>
+      <c r="AO25" s="7" t="s">
         <v>1131</v>
       </c>
-      <c r="AO25" s="7" t="s">
+      <c r="AP25" s="7" t="s">
         <v>1132</v>
       </c>
-      <c r="AP25" s="7" t="s">
+      <c r="AQ25" s="7" t="s">
         <v>1133</v>
-      </c>
-      <c r="AQ25" s="7" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="26" spans="1:43" ht="210" hidden="1">
       <c r="A26" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>676</v>
@@ -25055,22 +25044,22 @@
         <v>664</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="O26" s="7" t="s">
         <v>677</v>
       </c>
       <c r="P26" s="7" t="s">
+        <v>1135</v>
+      </c>
+      <c r="Q26" s="7" t="s">
         <v>1136</v>
       </c>
-      <c r="Q26" s="7" t="s">
+      <c r="R26" s="7" t="s">
         <v>1137</v>
       </c>
-      <c r="R26" s="7" t="s">
+      <c r="S26" s="7" t="s">
         <v>1138</v>
-      </c>
-      <c r="S26" s="7" t="s">
-        <v>1139</v>
       </c>
       <c r="T26" s="7" t="s">
         <v>46</v>
@@ -25133,21 +25122,21 @@
         <v>46</v>
       </c>
       <c r="AN26" s="7" t="s">
+        <v>1139</v>
+      </c>
+      <c r="AO26" s="7" t="s">
         <v>1140</v>
       </c>
-      <c r="AO26" s="7" t="s">
+      <c r="AP26" s="7" t="s">
         <v>1141</v>
       </c>
-      <c r="AP26" s="7" t="s">
+      <c r="AQ26" s="7" t="s">
         <v>1142</v>
-      </c>
-      <c r="AQ26" s="7" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="27" spans="1:43" ht="195" hidden="1">
       <c r="A27" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>680</v>
@@ -25186,22 +25175,22 @@
         <v>664</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="O27" s="7" t="s">
         <v>677</v>
       </c>
       <c r="P27" s="7" t="s">
+        <v>1144</v>
+      </c>
+      <c r="Q27" s="7" t="s">
         <v>1145</v>
       </c>
-      <c r="Q27" s="7" t="s">
+      <c r="R27" s="7" t="s">
         <v>1146</v>
       </c>
-      <c r="R27" s="7" t="s">
+      <c r="S27" s="7" t="s">
         <v>1147</v>
-      </c>
-      <c r="S27" s="7" t="s">
-        <v>1148</v>
       </c>
       <c r="T27" s="7" t="s">
         <v>46</v>
@@ -25264,21 +25253,21 @@
         <v>46</v>
       </c>
       <c r="AN27" s="7" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AO27" s="7" t="s">
         <v>1149</v>
       </c>
-      <c r="AO27" s="7" t="s">
+      <c r="AP27" s="7" t="s">
         <v>1150</v>
       </c>
-      <c r="AP27" s="7" t="s">
+      <c r="AQ27" s="7" t="s">
         <v>1151</v>
-      </c>
-      <c r="AQ27" s="7" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="28" spans="1:43" ht="180" hidden="1">
       <c r="A28" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>683</v>
@@ -25317,22 +25306,22 @@
         <v>664</v>
       </c>
       <c r="N28" s="7" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="O28" s="7" t="s">
         <v>684</v>
       </c>
       <c r="P28" s="7" t="s">
+        <v>1153</v>
+      </c>
+      <c r="Q28" s="7" t="s">
         <v>1154</v>
       </c>
-      <c r="Q28" s="7" t="s">
+      <c r="R28" s="7" t="s">
         <v>1155</v>
       </c>
-      <c r="R28" s="7" t="s">
+      <c r="S28" s="7" t="s">
         <v>1156</v>
-      </c>
-      <c r="S28" s="7" t="s">
-        <v>1157</v>
       </c>
       <c r="T28" s="7" t="s">
         <v>46</v>
@@ -25395,21 +25384,21 @@
         <v>46</v>
       </c>
       <c r="AN28" s="7" t="s">
+        <v>1157</v>
+      </c>
+      <c r="AO28" s="7" t="s">
         <v>1158</v>
       </c>
-      <c r="AO28" s="7" t="s">
+      <c r="AP28" s="7" t="s">
         <v>1159</v>
       </c>
-      <c r="AP28" s="7" t="s">
+      <c r="AQ28" s="7" t="s">
         <v>1160</v>
-      </c>
-      <c r="AQ28" s="7" t="s">
-        <v>1161</v>
       </c>
     </row>
     <row r="29" spans="1:43" ht="150" hidden="1">
       <c r="A29" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>687</v>
@@ -25448,22 +25437,22 @@
         <v>664</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="O29" s="7" t="s">
         <v>688</v>
       </c>
       <c r="P29" s="7" t="s">
+        <v>1162</v>
+      </c>
+      <c r="Q29" s="7" t="s">
         <v>1163</v>
       </c>
-      <c r="Q29" s="7" t="s">
+      <c r="R29" s="7" t="s">
         <v>1164</v>
       </c>
-      <c r="R29" s="7" t="s">
+      <c r="S29" s="7" t="s">
         <v>1165</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>1166</v>
       </c>
       <c r="T29" s="7" t="s">
         <v>46</v>
@@ -25526,21 +25515,21 @@
         <v>46</v>
       </c>
       <c r="AN29" s="7" t="s">
+        <v>1166</v>
+      </c>
+      <c r="AO29" s="7" t="s">
         <v>1167</v>
       </c>
-      <c r="AO29" s="7" t="s">
+      <c r="AP29" s="7" t="s">
         <v>1168</v>
       </c>
-      <c r="AP29" s="7" t="s">
+      <c r="AQ29" s="7" t="s">
         <v>1169</v>
-      </c>
-      <c r="AQ29" s="7" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="30" spans="1:43" ht="165" hidden="1">
       <c r="A30" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>691</v>
@@ -25579,22 +25568,22 @@
         <v>664</v>
       </c>
       <c r="N30" s="7" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="O30" s="7" t="s">
         <v>692</v>
       </c>
       <c r="P30" s="7" t="s">
+        <v>1171</v>
+      </c>
+      <c r="Q30" s="7" t="s">
         <v>1172</v>
       </c>
-      <c r="Q30" s="7" t="s">
+      <c r="R30" s="7" t="s">
         <v>1173</v>
       </c>
-      <c r="R30" s="7" t="s">
+      <c r="S30" s="7" t="s">
         <v>1174</v>
-      </c>
-      <c r="S30" s="7" t="s">
-        <v>1175</v>
       </c>
       <c r="T30" s="7" t="s">
         <v>46</v>
@@ -25657,21 +25646,21 @@
         <v>46</v>
       </c>
       <c r="AN30" s="7" t="s">
+        <v>1175</v>
+      </c>
+      <c r="AO30" s="7" t="s">
         <v>1176</v>
       </c>
-      <c r="AO30" s="7" t="s">
+      <c r="AP30" s="7" t="s">
         <v>1177</v>
       </c>
-      <c r="AP30" s="7" t="s">
+      <c r="AQ30" s="7" t="s">
         <v>1178</v>
-      </c>
-      <c r="AQ30" s="7" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="31" spans="1:43" ht="330" hidden="1">
       <c r="A31" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>232</v>
@@ -25710,10 +25699,10 @@
         <v>46</v>
       </c>
       <c r="N31" s="7" t="s">
+        <v>1179</v>
+      </c>
+      <c r="O31" s="7" t="s">
         <v>1180</v>
-      </c>
-      <c r="O31" s="7" t="s">
-        <v>1181</v>
       </c>
       <c r="P31" s="7" t="s">
         <v>46</v>
@@ -25761,7 +25750,7 @@
         <v>243</v>
       </c>
       <c r="AE31" s="7" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="AF31" s="7" t="s">
         <v>46</v>
@@ -25785,13 +25774,13 @@
         <v>46</v>
       </c>
       <c r="AM31" s="7" t="s">
+        <v>1182</v>
+      </c>
+      <c r="AN31" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AO31" s="7" t="s">
         <v>1183</v>
-      </c>
-      <c r="AN31" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AO31" s="7" t="s">
-        <v>1184</v>
       </c>
       <c r="AP31" s="7" t="s">
         <v>248</v>
@@ -25802,7 +25791,7 @@
     </row>
     <row r="32" spans="1:43" ht="105" hidden="1">
       <c r="A32" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>695</v>
@@ -25841,22 +25830,22 @@
         <v>46</v>
       </c>
       <c r="N32" s="7" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="O32" s="7" t="s">
         <v>701</v>
       </c>
       <c r="P32" s="7" t="s">
+        <v>1185</v>
+      </c>
+      <c r="Q32" s="7" t="s">
         <v>1186</v>
       </c>
-      <c r="Q32" s="7" t="s">
+      <c r="R32" s="7" t="s">
         <v>1187</v>
       </c>
-      <c r="R32" s="7" t="s">
+      <c r="S32" s="7" t="s">
         <v>1188</v>
-      </c>
-      <c r="S32" s="7" t="s">
-        <v>1189</v>
       </c>
       <c r="T32" s="7" t="s">
         <v>276</v>
@@ -25922,7 +25911,7 @@
         <v>46</v>
       </c>
       <c r="AO32" s="7" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="AP32" s="7" t="s">
         <v>46</v>
@@ -25933,7 +25922,7 @@
     </row>
     <row r="33" spans="1:43" ht="195" hidden="1">
       <c r="A33" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>696</v>
@@ -25972,22 +25961,22 @@
         <v>46</v>
       </c>
       <c r="N33" s="7" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="O33" s="7" t="s">
         <v>703</v>
       </c>
       <c r="P33" s="7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="Q33" s="7" t="s">
         <v>1192</v>
       </c>
-      <c r="Q33" s="7" t="s">
+      <c r="R33" s="7" t="s">
         <v>1193</v>
       </c>
-      <c r="R33" s="7" t="s">
+      <c r="S33" s="7" t="s">
         <v>1194</v>
-      </c>
-      <c r="S33" s="7" t="s">
-        <v>1195</v>
       </c>
       <c r="T33" s="7" t="s">
         <v>276</v>
@@ -26053,7 +26042,7 @@
         <v>46</v>
       </c>
       <c r="AO33" s="7" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="AP33" s="7" t="s">
         <v>46</v>
@@ -26064,7 +26053,7 @@
     </row>
     <row r="34" spans="1:43" ht="195" hidden="1">
       <c r="A34" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>697</v>
@@ -26103,22 +26092,22 @@
         <v>46</v>
       </c>
       <c r="N34" s="7" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="O34" s="7" t="s">
         <v>705</v>
       </c>
       <c r="P34" s="7" t="s">
+        <v>1197</v>
+      </c>
+      <c r="Q34" s="7" t="s">
         <v>1198</v>
       </c>
-      <c r="Q34" s="7" t="s">
-        <v>1199</v>
-      </c>
       <c r="R34" s="7" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="S34" s="7" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="T34" s="7" t="s">
         <v>276</v>
@@ -26184,7 +26173,7 @@
         <v>46</v>
       </c>
       <c r="AO34" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="AP34" s="7" t="s">
         <v>46</v>
@@ -26195,7 +26184,7 @@
     </row>
     <row r="35" spans="1:43" ht="120" hidden="1">
       <c r="A35" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>698</v>
@@ -26234,22 +26223,22 @@
         <v>46</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="O35" s="7" t="s">
         <v>708</v>
       </c>
       <c r="P35" s="7" t="s">
+        <v>1201</v>
+      </c>
+      <c r="Q35" s="7" t="s">
         <v>1202</v>
       </c>
-      <c r="Q35" s="7" t="s">
+      <c r="R35" s="7" t="s">
         <v>1203</v>
       </c>
-      <c r="R35" s="7" t="s">
+      <c r="S35" s="7" t="s">
         <v>1204</v>
-      </c>
-      <c r="S35" s="7" t="s">
-        <v>1205</v>
       </c>
       <c r="T35" s="7" t="s">
         <v>276</v>
@@ -26321,12 +26310,12 @@
         <v>46</v>
       </c>
       <c r="AQ35" s="7" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="36" spans="1:43" ht="135" hidden="1">
       <c r="A36" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>709</v>
@@ -26365,22 +26354,22 @@
         <v>46</v>
       </c>
       <c r="N36" s="7" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="O36" s="7" t="s">
         <v>710</v>
       </c>
       <c r="P36" s="7" t="s">
+        <v>1207</v>
+      </c>
+      <c r="Q36" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="Q36" s="7" t="s">
+      <c r="R36" s="7" t="s">
         <v>1209</v>
       </c>
-      <c r="R36" s="7" t="s">
+      <c r="S36" s="7" t="s">
         <v>1210</v>
-      </c>
-      <c r="S36" s="7" t="s">
-        <v>1211</v>
       </c>
       <c r="T36" s="7" t="s">
         <v>276</v>
@@ -26452,12 +26441,12 @@
         <v>46</v>
       </c>
       <c r="AQ36" s="7" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="37" spans="1:43" ht="135" hidden="1">
       <c r="A37" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B37" s="7" t="s">
         <v>711</v>
@@ -26496,22 +26485,22 @@
         <v>46</v>
       </c>
       <c r="N37" s="7" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="O37" s="7" t="s">
         <v>712</v>
       </c>
       <c r="P37" s="7" t="s">
+        <v>1213</v>
+      </c>
+      <c r="Q37" s="7" t="s">
         <v>1214</v>
       </c>
-      <c r="Q37" s="7" t="s">
+      <c r="R37" s="7" t="s">
         <v>1215</v>
       </c>
-      <c r="R37" s="7" t="s">
+      <c r="S37" s="7" t="s">
         <v>1216</v>
-      </c>
-      <c r="S37" s="7" t="s">
-        <v>1217</v>
       </c>
       <c r="T37" s="7" t="s">
         <v>276</v>
@@ -26583,12 +26572,12 @@
         <v>46</v>
       </c>
       <c r="AQ37" s="7" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="38" spans="1:43" ht="135" hidden="1">
       <c r="A38" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>713</v>
@@ -26627,22 +26616,22 @@
         <v>46</v>
       </c>
       <c r="N38" s="7" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="O38" s="7" t="s">
         <v>714</v>
       </c>
       <c r="P38" s="7" t="s">
+        <v>1219</v>
+      </c>
+      <c r="Q38" s="7" t="s">
         <v>1220</v>
       </c>
-      <c r="Q38" s="7" t="s">
+      <c r="R38" s="7" t="s">
         <v>1221</v>
       </c>
-      <c r="R38" s="7" t="s">
+      <c r="S38" s="7" t="s">
         <v>1222</v>
-      </c>
-      <c r="S38" s="7" t="s">
-        <v>1223</v>
       </c>
       <c r="T38" s="7" t="s">
         <v>276</v>
@@ -26714,12 +26703,12 @@
         <v>46</v>
       </c>
       <c r="AQ38" s="7" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="39" spans="1:43" ht="135" hidden="1">
       <c r="A39" s="1" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>715</v>
@@ -26758,22 +26747,22 @@
         <v>46</v>
       </c>
       <c r="N39" s="7" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="O39" s="7" t="s">
         <v>716</v>
       </c>
       <c r="P39" s="7" t="s">
+        <v>1225</v>
+      </c>
+      <c r="Q39" s="7" t="s">
         <v>1226</v>
       </c>
-      <c r="Q39" s="7" t="s">
+      <c r="R39" s="7" t="s">
         <v>1227</v>
       </c>
-      <c r="R39" s="7" t="s">
+      <c r="S39" s="7" t="s">
         <v>1228</v>
-      </c>
-      <c r="S39" s="7" t="s">
-        <v>1229</v>
       </c>
       <c r="T39" s="7" t="s">
         <v>276</v>
@@ -26845,12 +26834,12 @@
         <v>46</v>
       </c>
       <c r="AQ39" s="7" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="40" spans="1:43" ht="150" hidden="1">
       <c r="A40" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>717</v>
@@ -26889,22 +26878,22 @@
         <v>46</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="O40" s="7" t="s">
         <v>718</v>
       </c>
       <c r="P40" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="Q40" s="7" t="s">
         <v>1232</v>
       </c>
-      <c r="Q40" s="7" t="s">
+      <c r="R40" s="7" t="s">
         <v>1233</v>
       </c>
-      <c r="R40" s="7" t="s">
+      <c r="S40" s="7" t="s">
         <v>1234</v>
-      </c>
-      <c r="S40" s="7" t="s">
-        <v>1235</v>
       </c>
       <c r="T40" s="7" t="s">
         <v>276</v>
@@ -26976,12 +26965,12 @@
         <v>46</v>
       </c>
       <c r="AQ40" s="7" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="41" spans="1:43" ht="150" hidden="1">
       <c r="A41" s="4" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>249</v>
@@ -27112,7 +27101,7 @@
     </row>
     <row r="42" spans="1:43" ht="90" hidden="1">
       <c r="A42" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>261</v>
@@ -27151,22 +27140,22 @@
         <v>267</v>
       </c>
       <c r="N42" s="7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="O42" s="7" t="s">
         <v>1237</v>
       </c>
-      <c r="O42" s="7" t="s">
+      <c r="P42" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q42" s="7" t="s">
         <v>1238</v>
       </c>
-      <c r="P42" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q42" s="7" t="s">
+      <c r="R42" s="7" t="s">
         <v>1239</v>
       </c>
-      <c r="R42" s="7" t="s">
+      <c r="S42" s="7" t="s">
         <v>1240</v>
-      </c>
-      <c r="S42" s="7" t="s">
-        <v>1241</v>
       </c>
       <c r="T42" s="7" t="s">
         <v>268</v>
@@ -27229,21 +27218,21 @@
         <v>46</v>
       </c>
       <c r="AN42" s="7" t="s">
+        <v>1241</v>
+      </c>
+      <c r="AO42" s="7" t="s">
         <v>1242</v>
       </c>
-      <c r="AO42" s="7" t="s">
+      <c r="AP42" s="7" t="s">
         <v>1243</v>
       </c>
-      <c r="AP42" s="7" t="s">
+      <c r="AQ42" s="7" t="s">
         <v>1244</v>
-      </c>
-      <c r="AQ42" s="7" t="s">
-        <v>1245</v>
       </c>
     </row>
     <row r="43" spans="1:43" ht="150" hidden="1">
       <c r="A43" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>719</v>
@@ -27282,7 +27271,7 @@
         <v>722</v>
       </c>
       <c r="N43" s="7" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="O43" s="7" t="s">
         <v>725</v>
@@ -27291,13 +27280,13 @@
         <v>46</v>
       </c>
       <c r="Q43" s="14" t="s">
+        <v>1246</v>
+      </c>
+      <c r="R43" s="7" t="s">
         <v>1247</v>
       </c>
-      <c r="R43" s="7" t="s">
+      <c r="S43" s="14" t="s">
         <v>1248</v>
-      </c>
-      <c r="S43" s="14" t="s">
-        <v>1249</v>
       </c>
       <c r="T43" s="7" t="s">
         <v>46</v>
@@ -27374,7 +27363,7 @@
     </row>
     <row r="44" spans="1:43" ht="150" hidden="1">
       <c r="A44" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>726</v>
@@ -27413,7 +27402,7 @@
         <v>722</v>
       </c>
       <c r="N44" s="7" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="O44" s="7" t="s">
         <v>727</v>
@@ -27422,13 +27411,13 @@
         <v>46</v>
       </c>
       <c r="Q44" s="14" t="s">
+        <v>1250</v>
+      </c>
+      <c r="R44" s="7" t="s">
         <v>1251</v>
       </c>
-      <c r="R44" s="7" t="s">
+      <c r="S44" s="14" t="s">
         <v>1252</v>
-      </c>
-      <c r="S44" s="14" t="s">
-        <v>1253</v>
       </c>
       <c r="T44" s="7" t="s">
         <v>46</v>
@@ -27505,7 +27494,7 @@
     </row>
     <row r="45" spans="1:43" ht="150" hidden="1">
       <c r="A45" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>730</v>
@@ -27544,7 +27533,7 @@
         <v>722</v>
       </c>
       <c r="N45" s="7" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="O45" s="7" t="s">
         <v>731</v>
@@ -27553,13 +27542,13 @@
         <v>46</v>
       </c>
       <c r="Q45" s="14" t="s">
+        <v>1254</v>
+      </c>
+      <c r="R45" s="7" t="s">
         <v>1255</v>
       </c>
-      <c r="R45" s="7" t="s">
+      <c r="S45" s="14" t="s">
         <v>1256</v>
-      </c>
-      <c r="S45" s="14" t="s">
-        <v>1257</v>
       </c>
       <c r="T45" s="7" t="s">
         <v>46</v>
@@ -27628,7 +27617,7 @@
         <v>46</v>
       </c>
       <c r="AP45" s="7" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="AQ45" s="7" t="s">
         <v>736</v>
@@ -27636,7 +27625,7 @@
     </row>
     <row r="46" spans="1:43" ht="150" hidden="1">
       <c r="A46" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>732</v>
@@ -27675,7 +27664,7 @@
         <v>722</v>
       </c>
       <c r="N46" s="7" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="O46" s="7" t="s">
         <v>738</v>
@@ -27684,13 +27673,13 @@
         <v>46</v>
       </c>
       <c r="Q46" s="14" t="s">
+        <v>1259</v>
+      </c>
+      <c r="R46" s="7" t="s">
         <v>1260</v>
       </c>
-      <c r="R46" s="7" t="s">
+      <c r="S46" s="14" t="s">
         <v>1261</v>
-      </c>
-      <c r="S46" s="14" t="s">
-        <v>1262</v>
       </c>
       <c r="T46" s="7" t="s">
         <v>46</v>
@@ -27759,15 +27748,15 @@
         <v>46</v>
       </c>
       <c r="AP46" s="7" t="s">
+        <v>1262</v>
+      </c>
+      <c r="AQ46" s="7" t="s">
         <v>1263</v>
-      </c>
-      <c r="AQ46" s="7" t="s">
-        <v>1264</v>
       </c>
     </row>
     <row r="47" spans="1:43" ht="150" hidden="1">
       <c r="A47" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>740</v>
@@ -27806,7 +27795,7 @@
         <v>722</v>
       </c>
       <c r="N47" s="7" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="O47" s="7" t="s">
         <v>742</v>
@@ -27815,13 +27804,13 @@
         <v>46</v>
       </c>
       <c r="Q47" s="14" t="s">
+        <v>1265</v>
+      </c>
+      <c r="R47" s="7" t="s">
         <v>1266</v>
       </c>
-      <c r="R47" s="7" t="s">
+      <c r="S47" s="14" t="s">
         <v>1267</v>
-      </c>
-      <c r="S47" s="14" t="s">
-        <v>1268</v>
       </c>
       <c r="T47" s="7" t="s">
         <v>46</v>
@@ -27890,7 +27879,7 @@
         <v>46</v>
       </c>
       <c r="AP47" s="7" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="AQ47" s="7" t="s">
         <v>744</v>
@@ -27898,7 +27887,7 @@
     </row>
     <row r="48" spans="1:43" ht="150" hidden="1">
       <c r="A48" s="1" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>745</v>
@@ -27937,7 +27926,7 @@
         <v>722</v>
       </c>
       <c r="N48" s="7" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="O48" s="7" t="s">
         <v>746</v>
@@ -27946,13 +27935,13 @@
         <v>46</v>
       </c>
       <c r="Q48" s="14" t="s">
+        <v>1270</v>
+      </c>
+      <c r="R48" s="7" t="s">
         <v>1271</v>
       </c>
-      <c r="R48" s="7" t="s">
+      <c r="S48" s="14" t="s">
         <v>1272</v>
-      </c>
-      <c r="S48" s="14" t="s">
-        <v>1273</v>
       </c>
       <c r="T48" s="7" t="s">
         <v>46</v>
@@ -28021,7 +28010,7 @@
         <v>46</v>
       </c>
       <c r="AP48" s="7" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="AQ48" s="7" t="s">
         <v>748</v>
@@ -28029,7 +28018,7 @@
     </row>
     <row r="49" spans="1:43" ht="90" hidden="1" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>749</v>
@@ -28068,7 +28057,7 @@
         <v>722</v>
       </c>
       <c r="N49" s="7" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="O49" s="7" t="s">
         <v>750</v>
@@ -28077,13 +28066,13 @@
         <v>46</v>
       </c>
       <c r="Q49" s="14" t="s">
+        <v>1275</v>
+      </c>
+      <c r="R49" s="7" t="s">
         <v>1276</v>
       </c>
-      <c r="R49" s="7" t="s">
+      <c r="S49" s="14" t="s">
         <v>1277</v>
-      </c>
-      <c r="S49" s="14" t="s">
-        <v>1278</v>
       </c>
       <c r="T49" s="7" t="s">
         <v>46</v>
@@ -28152,7 +28141,7 @@
         <v>46</v>
       </c>
       <c r="AP49" s="7" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="AQ49" s="7" t="s">
         <v>752</v>
@@ -28160,7 +28149,7 @@
     </row>
     <row r="50" spans="1:43" ht="75" hidden="1" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>753</v>
@@ -28199,7 +28188,7 @@
         <v>722</v>
       </c>
       <c r="N50" s="7" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="O50" s="7" t="s">
         <v>754</v>
@@ -28208,13 +28197,13 @@
         <v>46</v>
       </c>
       <c r="Q50" s="14" t="s">
+        <v>1280</v>
+      </c>
+      <c r="R50" s="7" t="s">
         <v>1281</v>
       </c>
-      <c r="R50" s="7" t="s">
+      <c r="S50" s="14" t="s">
         <v>1282</v>
-      </c>
-      <c r="S50" s="14" t="s">
-        <v>1283</v>
       </c>
       <c r="T50" s="7" t="s">
         <v>46</v>
@@ -28283,7 +28272,7 @@
         <v>46</v>
       </c>
       <c r="AP50" s="7" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="AQ50" s="7" t="s">
         <v>756</v>
@@ -28291,7 +28280,7 @@
     </row>
     <row r="51" spans="1:43" ht="120" hidden="1" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>757</v>
@@ -28330,7 +28319,7 @@
         <v>722</v>
       </c>
       <c r="N51" s="7" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="O51" s="7" t="s">
         <v>758</v>
@@ -28339,13 +28328,13 @@
         <v>46</v>
       </c>
       <c r="Q51" s="14" t="s">
+        <v>1285</v>
+      </c>
+      <c r="R51" s="7" t="s">
         <v>1286</v>
       </c>
-      <c r="R51" s="7" t="s">
+      <c r="S51" s="14" t="s">
         <v>1287</v>
-      </c>
-      <c r="S51" s="14" t="s">
-        <v>1288</v>
       </c>
       <c r="T51" s="7" t="s">
         <v>46</v>
@@ -28422,7 +28411,7 @@
     </row>
     <row r="52" spans="1:43" ht="210" hidden="1" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>277</v>
@@ -28461,16 +28450,16 @@
         <v>46</v>
       </c>
       <c r="N52" s="7" t="s">
+        <v>1288</v>
+      </c>
+      <c r="O52" s="7" t="s">
         <v>1289</v>
       </c>
-      <c r="O52" s="7" t="s">
+      <c r="P52" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q52" s="7" t="s">
         <v>1290</v>
-      </c>
-      <c r="P52" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q52" s="7" t="s">
-        <v>1291</v>
       </c>
       <c r="R52" s="7" t="s">
         <v>46</v>
@@ -28545,7 +28534,7 @@
         <v>46</v>
       </c>
       <c r="AP52" s="7" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="AQ52" s="7" t="s">
         <v>46</v>
@@ -28553,7 +28542,7 @@
     </row>
     <row r="53" spans="1:43" ht="120" hidden="1" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>47</v>
@@ -28684,7 +28673,7 @@
     </row>
     <row r="54" spans="1:43" ht="180" hidden="1" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>288</v>
@@ -28732,10 +28721,10 @@
         <v>46</v>
       </c>
       <c r="Q54" s="7" t="s">
+        <v>1292</v>
+      </c>
+      <c r="R54" s="7" t="s">
         <v>1293</v>
-      </c>
-      <c r="R54" s="7" t="s">
-        <v>1294</v>
       </c>
       <c r="S54" s="7" t="s">
         <v>46</v>
@@ -28815,7 +28804,7 @@
     </row>
     <row r="55" spans="1:43" ht="120" hidden="1">
       <c r="A55" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>305</v>
@@ -28854,22 +28843,22 @@
         <v>46</v>
       </c>
       <c r="N55" s="7" t="s">
+        <v>1294</v>
+      </c>
+      <c r="O55" s="7" t="s">
         <v>1295</v>
       </c>
-      <c r="O55" s="7" t="s">
+      <c r="P55" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q55" s="7" t="s">
         <v>1296</v>
       </c>
-      <c r="P55" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q55" s="7" t="s">
+      <c r="R55" s="7" t="s">
         <v>1297</v>
       </c>
-      <c r="R55" s="7" t="s">
+      <c r="S55" s="7" t="s">
         <v>1298</v>
-      </c>
-      <c r="S55" s="7" t="s">
-        <v>1299</v>
       </c>
       <c r="T55" s="7" t="s">
         <v>46</v>
@@ -28935,10 +28924,10 @@
         <v>46</v>
       </c>
       <c r="AO55" s="7" t="s">
+        <v>1299</v>
+      </c>
+      <c r="AP55" s="7" t="s">
         <v>1300</v>
-      </c>
-      <c r="AP55" s="7" t="s">
-        <v>1301</v>
       </c>
       <c r="AQ55" s="7" t="s">
         <v>46</v>
@@ -28946,7 +28935,7 @@
     </row>
     <row r="56" spans="1:43" ht="210" hidden="1">
       <c r="A56" s="1" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>314</v>
@@ -28985,22 +28974,22 @@
         <v>46</v>
       </c>
       <c r="N56" s="7" t="s">
+        <v>1301</v>
+      </c>
+      <c r="O56" s="7" t="s">
         <v>1302</v>
       </c>
-      <c r="O56" s="7" t="s">
+      <c r="P56" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q56" s="7" t="s">
         <v>1303</v>
       </c>
-      <c r="P56" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q56" s="7" t="s">
+      <c r="R56" s="7" t="s">
         <v>1304</v>
       </c>
-      <c r="R56" s="7" t="s">
+      <c r="S56" s="7" t="s">
         <v>1305</v>
-      </c>
-      <c r="S56" s="7" t="s">
-        <v>1306</v>
       </c>
       <c r="T56" s="7" t="s">
         <v>319</v>
@@ -29027,16 +29016,16 @@
         <v>46</v>
       </c>
       <c r="AB56" s="7" t="s">
+        <v>1306</v>
+      </c>
+      <c r="AC56" s="7" t="s">
         <v>1307</v>
       </c>
-      <c r="AC56" s="7" t="s">
+      <c r="AD56" s="7" t="s">
         <v>1308</v>
       </c>
-      <c r="AD56" s="7" t="s">
+      <c r="AE56" s="7" t="s">
         <v>1309</v>
-      </c>
-      <c r="AE56" s="7" t="s">
-        <v>1310</v>
       </c>
       <c r="AF56" s="7" t="s">
         <v>46</v>
@@ -29069,7 +29058,7 @@
         <v>46</v>
       </c>
       <c r="AP56" s="7" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="AQ56" s="7" t="s">
         <v>46</v>
@@ -29077,7 +29066,7 @@
     </row>
     <row r="57" spans="1:43" ht="120" hidden="1">
       <c r="A57" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>325</v>
@@ -29116,10 +29105,10 @@
         <v>46</v>
       </c>
       <c r="N57" s="7" t="s">
+        <v>1311</v>
+      </c>
+      <c r="O57" s="7" t="s">
         <v>1312</v>
-      </c>
-      <c r="O57" s="7" t="s">
-        <v>1313</v>
       </c>
       <c r="P57" s="7" t="s">
         <v>46</v>
@@ -29208,7 +29197,7 @@
     </row>
     <row r="58" spans="1:43" ht="180" hidden="1">
       <c r="A58" s="1" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>352</v>
@@ -29298,7 +29287,7 @@
         <v>46</v>
       </c>
       <c r="AE58" s="7" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="AF58" s="7" t="s">
         <v>46</v>
@@ -29322,7 +29311,7 @@
         <v>46</v>
       </c>
       <c r="AM58" s="7" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="AN58" s="7" t="s">
         <v>46</v>
@@ -29339,7 +29328,7 @@
     </row>
     <row r="59" spans="1:43" ht="75" hidden="1">
       <c r="A59" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>336</v>
@@ -29351,7 +29340,7 @@
         <v>48</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="F59" s="7">
         <v>185</v>
@@ -29459,7 +29448,7 @@
         <v>276</v>
       </c>
       <c r="AO59" s="7" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="AP59" s="7" t="s">
         <v>46</v>
@@ -29470,7 +29459,7 @@
     </row>
     <row r="60" spans="1:43" ht="195" hidden="1">
       <c r="A60" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>81</v>
@@ -29509,19 +29498,19 @@
         <v>46</v>
       </c>
       <c r="N60" s="7" t="s">
+        <v>1317</v>
+      </c>
+      <c r="O60" s="7" t="s">
         <v>1318</v>
       </c>
-      <c r="O60" s="7" t="s">
+      <c r="P60" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q60" s="7" t="s">
         <v>1319</v>
       </c>
-      <c r="P60" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q60" s="7" t="s">
+      <c r="R60" s="7" t="s">
         <v>1320</v>
-      </c>
-      <c r="R60" s="7" t="s">
-        <v>1321</v>
       </c>
       <c r="S60" s="7" t="s">
         <v>46</v>
@@ -29601,7 +29590,7 @@
     </row>
     <row r="61" spans="1:43" ht="135" hidden="1">
       <c r="A61" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>359</v>
@@ -29640,22 +29629,22 @@
         <v>365</v>
       </c>
       <c r="N61" s="7" t="s">
+        <v>1321</v>
+      </c>
+      <c r="O61" s="7" t="s">
         <v>1322</v>
       </c>
-      <c r="O61" s="7" t="s">
+      <c r="P61" s="7" t="s">
         <v>1323</v>
       </c>
-      <c r="P61" s="7" t="s">
+      <c r="Q61" s="7" t="s">
         <v>1324</v>
       </c>
-      <c r="Q61" s="7" t="s">
+      <c r="R61" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S61" s="7" t="s">
         <v>1325</v>
-      </c>
-      <c r="R61" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S61" s="7" t="s">
-        <v>1326</v>
       </c>
       <c r="T61" s="7" t="s">
         <v>46</v>
@@ -29721,18 +29710,18 @@
         <v>46</v>
       </c>
       <c r="AO61" s="7" t="s">
+        <v>1326</v>
+      </c>
+      <c r="AP61" s="7" t="s">
         <v>1327</v>
       </c>
-      <c r="AP61" s="7" t="s">
+      <c r="AQ61" s="7" t="s">
         <v>1328</v>
-      </c>
-      <c r="AQ61" s="7" t="s">
-        <v>1329</v>
       </c>
     </row>
     <row r="62" spans="1:43" ht="210" hidden="1">
       <c r="A62" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>369</v>
@@ -29771,10 +29760,10 @@
         <v>46</v>
       </c>
       <c r="N62" s="7" t="s">
+        <v>1329</v>
+      </c>
+      <c r="O62" s="7" t="s">
         <v>1330</v>
-      </c>
-      <c r="O62" s="7" t="s">
-        <v>1331</v>
       </c>
       <c r="P62" s="7" t="s">
         <v>46</v>
@@ -29863,7 +29852,7 @@
     </row>
     <row r="63" spans="1:43" ht="150" hidden="1">
       <c r="A63" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>386</v>
@@ -29902,16 +29891,16 @@
         <v>46</v>
       </c>
       <c r="N63" s="7" t="s">
+        <v>1331</v>
+      </c>
+      <c r="O63" s="7" t="s">
         <v>1332</v>
       </c>
-      <c r="O63" s="7" t="s">
+      <c r="P63" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q63" s="7" t="s">
         <v>1333</v>
-      </c>
-      <c r="P63" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q63" s="7" t="s">
-        <v>1334</v>
       </c>
       <c r="R63" s="7" t="s">
         <v>46</v>
@@ -29965,7 +29954,7 @@
         <v>396</v>
       </c>
       <c r="AI63" s="9" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="AJ63" s="7" t="s">
         <v>397</v>
@@ -29980,21 +29969,21 @@
         <v>46</v>
       </c>
       <c r="AN63" s="7" t="s">
+        <v>1335</v>
+      </c>
+      <c r="AO63" s="7" t="s">
         <v>1336</v>
       </c>
-      <c r="AO63" s="7" t="s">
+      <c r="AP63" s="7" t="s">
         <v>1337</v>
       </c>
-      <c r="AP63" s="7" t="s">
+      <c r="AQ63" s="7" t="s">
         <v>1338</v>
-      </c>
-      <c r="AQ63" s="7" t="s">
-        <v>1339</v>
       </c>
     </row>
     <row r="64" spans="1:43" ht="150" hidden="1">
       <c r="A64" s="4" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>817</v>
@@ -30134,7 +30123,7 @@
     </row>
     <row r="65" spans="1:43" ht="120" hidden="1">
       <c r="A65" s="1" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>94</v>
@@ -30173,19 +30162,19 @@
         <v>46</v>
       </c>
       <c r="N65" s="7" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="P65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q65" s="7" t="s">
         <v>1340</v>
       </c>
-      <c r="O65" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="P65" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q65" s="7" t="s">
+      <c r="R65" s="7" t="s">
         <v>1341</v>
-      </c>
-      <c r="R65" s="7" t="s">
-        <v>1342</v>
       </c>
       <c r="S65" s="7" t="s">
         <v>46</v>
@@ -30215,13 +30204,13 @@
         <v>46</v>
       </c>
       <c r="AB65" s="7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AC65" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD65" s="7" t="s">
         <v>1343</v>
-      </c>
-      <c r="AC65" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD65" s="7" t="s">
-        <v>1344</v>
       </c>
       <c r="AE65" s="7" t="s">
         <v>46</v>
@@ -30265,7 +30254,7 @@
     </row>
     <row r="66" spans="1:43" ht="150" hidden="1">
       <c r="A66" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>398</v>
@@ -30396,7 +30385,7 @@
     </row>
     <row r="67" spans="1:43" ht="105" hidden="1">
       <c r="A67" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>409</v>
@@ -30435,22 +30424,22 @@
         <v>46</v>
       </c>
       <c r="N67" s="7" t="s">
+        <v>1344</v>
+      </c>
+      <c r="O67" s="7" t="s">
         <v>1345</v>
       </c>
-      <c r="O67" s="7" t="s">
+      <c r="P67" s="7" t="s">
         <v>1346</v>
       </c>
-      <c r="P67" s="7" t="s">
+      <c r="Q67" s="7" t="s">
         <v>1347</v>
       </c>
-      <c r="Q67" s="7" t="s">
+      <c r="R67" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S67" s="7" t="s">
         <v>1348</v>
-      </c>
-      <c r="R67" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S67" s="7" t="s">
-        <v>1349</v>
       </c>
       <c r="T67" s="7" t="s">
         <v>46</v>
@@ -30527,7 +30516,7 @@
     </row>
     <row r="68" spans="1:43" ht="75" hidden="1">
       <c r="A68" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>421</v>
@@ -30658,7 +30647,7 @@
     </row>
     <row r="69" spans="1:43" ht="75" hidden="1">
       <c r="A69" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>433</v>
@@ -30784,12 +30773,12 @@
         <v>46</v>
       </c>
       <c r="AQ69" s="7" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="70" spans="1:43" ht="105" hidden="1">
       <c r="A70" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>447</v>
@@ -30828,7 +30817,7 @@
         <v>46</v>
       </c>
       <c r="N70" s="7" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="O70" s="7" t="s">
         <v>450</v>
@@ -30920,7 +30909,7 @@
     </row>
     <row r="71" spans="1:43" ht="105" hidden="1">
       <c r="A71" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>460</v>
@@ -31051,7 +31040,7 @@
     </row>
     <row r="72" spans="1:43" ht="135" hidden="1">
       <c r="A72" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>474</v>
@@ -31182,7 +31171,7 @@
     </row>
     <row r="73" spans="1:43" ht="120" hidden="1">
       <c r="A73" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>482</v>
@@ -31313,7 +31302,7 @@
     </row>
     <row r="74" spans="1:43" ht="105" hidden="1">
       <c r="A74" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>496</v>
@@ -31352,22 +31341,22 @@
         <v>46</v>
       </c>
       <c r="N74" s="7" t="s">
+        <v>1351</v>
+      </c>
+      <c r="O74" s="7" t="s">
         <v>1352</v>
       </c>
-      <c r="O74" s="7" t="s">
+      <c r="P74" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q74" s="7" t="s">
         <v>1353</v>
       </c>
-      <c r="P74" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q74" s="7" t="s">
+      <c r="R74" s="7" t="s">
         <v>1354</v>
       </c>
-      <c r="R74" s="7" t="s">
+      <c r="S74" s="7" t="s">
         <v>1355</v>
-      </c>
-      <c r="S74" s="7" t="s">
-        <v>1356</v>
       </c>
       <c r="T74" s="7" t="s">
         <v>501</v>
@@ -31444,7 +31433,7 @@
     </row>
     <row r="75" spans="1:43" ht="135" hidden="1">
       <c r="A75" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>513</v>
@@ -31483,22 +31472,22 @@
         <v>520</v>
       </c>
       <c r="N75" s="7" t="s">
+        <v>1356</v>
+      </c>
+      <c r="O75" s="7" t="s">
         <v>1357</v>
       </c>
-      <c r="O75" s="7" t="s">
+      <c r="P75" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q75" s="7" t="s">
         <v>1358</v>
       </c>
-      <c r="P75" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q75" s="7" t="s">
+      <c r="R75" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S75" s="7" t="s">
         <v>1359</v>
-      </c>
-      <c r="R75" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S75" s="7" t="s">
-        <v>1360</v>
       </c>
       <c r="T75" s="7" t="s">
         <v>521</v>
@@ -31564,18 +31553,18 @@
         <v>46</v>
       </c>
       <c r="AO75" s="7" t="s">
+        <v>1360</v>
+      </c>
+      <c r="AP75" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AQ75" s="7" t="s">
         <v>1361</v>
-      </c>
-      <c r="AP75" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ75" s="7" t="s">
-        <v>1362</v>
       </c>
     </row>
     <row r="76" spans="1:43" ht="90" hidden="1">
       <c r="A76" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>529</v>
@@ -31706,7 +31695,7 @@
     </row>
     <row r="77" spans="1:43" ht="135" hidden="1">
       <c r="A77" s="1" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>105</v>
@@ -31745,7 +31734,7 @@
         <v>102</v>
       </c>
       <c r="N77" s="7" t="s">
-        <v>1363</v>
+        <v>1362</v>
       </c>
       <c r="O77" s="7" t="s">
         <v>110</v>
@@ -31837,7 +31826,7 @@
     </row>
     <row r="78" spans="1:43" ht="150" hidden="1">
       <c r="A78" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>533</v>
@@ -31966,9 +31955,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:43" ht="81.75" hidden="1" customHeight="1">
+    <row r="79" spans="1:43" ht="81.75" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>64</v>
@@ -32007,7 +31996,7 @@
         <v>46</v>
       </c>
       <c r="N79" s="7" t="s">
-        <v>1364</v>
+        <v>1363</v>
       </c>
       <c r="O79" s="7" t="s">
         <v>70</v>
@@ -32066,8 +32055,8 @@
       <c r="AG79" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AH79" s="22" t="s">
-        <v>859</v>
+      <c r="AH79" s="13" t="s">
+        <v>1441</v>
       </c>
       <c r="AI79" s="9" t="s">
         <v>46</v>
@@ -32099,7 +32088,7 @@
     </row>
     <row r="80" spans="1:43" ht="90" hidden="1">
       <c r="A80" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>546</v>
@@ -32198,7 +32187,7 @@
         <v>46</v>
       </c>
       <c r="AH80" s="9" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="AI80" s="9" t="s">
         <v>46</v>
@@ -32230,7 +32219,7 @@
     </row>
     <row r="81" spans="1:43" ht="135" hidden="1">
       <c r="A81" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>554</v>
@@ -32269,19 +32258,19 @@
         <v>46</v>
       </c>
       <c r="N81" s="7" t="s">
+        <v>1365</v>
+      </c>
+      <c r="O81" s="7" t="s">
         <v>1366</v>
       </c>
-      <c r="O81" s="7" t="s">
+      <c r="P81" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q81" s="7" t="s">
         <v>1367</v>
       </c>
-      <c r="P81" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q81" s="7" t="s">
+      <c r="R81" s="7" t="s">
         <v>1368</v>
-      </c>
-      <c r="R81" s="7" t="s">
-        <v>1369</v>
       </c>
       <c r="S81" s="7" t="s">
         <v>46</v>
@@ -32329,10 +32318,10 @@
         <v>46</v>
       </c>
       <c r="AH81" s="9" t="s">
+        <v>1369</v>
+      </c>
+      <c r="AI81" s="9" t="s">
         <v>1370</v>
-      </c>
-      <c r="AI81" s="9" t="s">
-        <v>1371</v>
       </c>
       <c r="AJ81" s="7" t="s">
         <v>567</v>
@@ -32350,7 +32339,7 @@
         <v>46</v>
       </c>
       <c r="AO81" s="7" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="AP81" s="7" t="s">
         <v>46</v>
@@ -32361,7 +32350,7 @@
     </row>
     <row r="82" spans="1:43" ht="45" hidden="1">
       <c r="A82" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>568</v>
@@ -32400,10 +32389,10 @@
         <v>572</v>
       </c>
       <c r="N82" s="7" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O82" s="7" t="s">
         <v>1373</v>
-      </c>
-      <c r="O82" s="7" t="s">
-        <v>1374</v>
       </c>
       <c r="P82" s="7" t="s">
         <v>46</v>
@@ -32484,7 +32473,7 @@
         <v>46</v>
       </c>
       <c r="AP82" s="7" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="AQ82" s="7" t="s">
         <v>46</v>
@@ -32492,7 +32481,7 @@
     </row>
     <row r="83" spans="1:43" ht="75" hidden="1">
       <c r="A83" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>832</v>
@@ -32531,19 +32520,19 @@
         <v>46</v>
       </c>
       <c r="N83" s="7" t="s">
+        <v>1375</v>
+      </c>
+      <c r="O83" s="7" t="s">
         <v>1376</v>
       </c>
-      <c r="O83" s="7" t="s">
+      <c r="P83" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q83" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="R83" s="7" t="s">
         <v>1377</v>
-      </c>
-      <c r="P83" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q83" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="R83" s="7" t="s">
-        <v>1378</v>
       </c>
       <c r="S83" s="7" t="s">
         <v>46</v>
@@ -32609,7 +32598,7 @@
         <v>46</v>
       </c>
       <c r="AN83" s="7" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="AO83" s="7" t="s">
         <v>46</v>
@@ -32623,7 +32612,7 @@
     </row>
     <row r="84" spans="1:43" ht="90" hidden="1">
       <c r="A84" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>762</v>
@@ -32662,22 +32651,22 @@
         <v>767</v>
       </c>
       <c r="N84" s="7" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="O84" s="7" t="s">
         <v>768</v>
       </c>
       <c r="P84" s="7" t="s">
+        <v>1380</v>
+      </c>
+      <c r="Q84" s="7" t="s">
         <v>1381</v>
       </c>
-      <c r="Q84" s="7" t="s">
+      <c r="R84" s="7" t="s">
         <v>1382</v>
       </c>
-      <c r="R84" s="7" t="s">
+      <c r="S84" s="7" t="s">
         <v>1383</v>
-      </c>
-      <c r="S84" s="7" t="s">
-        <v>1384</v>
       </c>
       <c r="T84" s="7" t="s">
         <v>276</v>
@@ -32754,7 +32743,7 @@
     </row>
     <row r="85" spans="1:43" ht="90" hidden="1">
       <c r="A85" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>763</v>
@@ -32793,22 +32782,22 @@
         <v>767</v>
       </c>
       <c r="N85" s="7" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O85" s="7" t="s">
         <v>1385</v>
       </c>
-      <c r="O85" s="7" t="s">
+      <c r="P85" s="7" t="s">
         <v>1386</v>
       </c>
-      <c r="P85" s="7" t="s">
+      <c r="Q85" s="7" t="s">
         <v>1387</v>
       </c>
-      <c r="Q85" s="7" t="s">
+      <c r="R85" s="7" t="s">
         <v>1388</v>
       </c>
-      <c r="R85" s="7" t="s">
+      <c r="S85" s="7" t="s">
         <v>1389</v>
-      </c>
-      <c r="S85" s="7" t="s">
-        <v>1390</v>
       </c>
       <c r="T85" s="7" t="s">
         <v>276</v>
@@ -32885,7 +32874,7 @@
     </row>
     <row r="86" spans="1:43" ht="90" hidden="1">
       <c r="A86" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>764</v>
@@ -32924,22 +32913,22 @@
         <v>767</v>
       </c>
       <c r="N86" s="7" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="O86" s="7" t="s">
         <v>773</v>
       </c>
       <c r="P86" s="7" t="s">
+        <v>1391</v>
+      </c>
+      <c r="Q86" s="7" t="s">
         <v>1392</v>
       </c>
-      <c r="Q86" s="7" t="s">
+      <c r="R86" s="7" t="s">
         <v>1393</v>
       </c>
-      <c r="R86" s="7" t="s">
+      <c r="S86" s="7" t="s">
         <v>1394</v>
-      </c>
-      <c r="S86" s="7" t="s">
-        <v>1395</v>
       </c>
       <c r="T86" s="7" t="s">
         <v>276</v>
@@ -33016,7 +33005,7 @@
     </row>
     <row r="87" spans="1:43" ht="165" hidden="1">
       <c r="A87" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>765</v>
@@ -33055,22 +33044,22 @@
         <v>767</v>
       </c>
       <c r="N87" s="7" t="s">
-        <v>1396</v>
+        <v>1395</v>
       </c>
       <c r="O87" s="7" t="s">
         <v>776</v>
       </c>
       <c r="P87" s="7" t="s">
+        <v>1396</v>
+      </c>
+      <c r="Q87" s="7" t="s">
         <v>1397</v>
       </c>
-      <c r="Q87" s="7" t="s">
+      <c r="R87" s="7" t="s">
         <v>1398</v>
       </c>
-      <c r="R87" s="7" t="s">
+      <c r="S87" s="7" t="s">
         <v>1399</v>
-      </c>
-      <c r="S87" s="7" t="s">
-        <v>1400</v>
       </c>
       <c r="T87" s="7" t="s">
         <v>276</v>
@@ -33136,7 +33125,7 @@
         <v>771</v>
       </c>
       <c r="AO87" s="7" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="AP87" s="16">
         <v>0.05</v>
@@ -33147,7 +33136,7 @@
     </row>
     <row r="88" spans="1:43" ht="90" hidden="1">
       <c r="A88" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>779</v>
@@ -33186,22 +33175,22 @@
         <v>767</v>
       </c>
       <c r="N88" s="7" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="O88" s="7" t="s">
         <v>780</v>
       </c>
       <c r="P88" s="7" t="s">
+        <v>1402</v>
+      </c>
+      <c r="Q88" s="7" t="s">
         <v>1403</v>
       </c>
-      <c r="Q88" s="7" t="s">
+      <c r="R88" s="7" t="s">
         <v>1404</v>
       </c>
-      <c r="R88" s="7" t="s">
+      <c r="S88" s="7" t="s">
         <v>1405</v>
-      </c>
-      <c r="S88" s="7" t="s">
-        <v>1406</v>
       </c>
       <c r="T88" s="7" t="s">
         <v>276</v>
@@ -33278,7 +33267,7 @@
     </row>
     <row r="89" spans="1:43" ht="105" hidden="1">
       <c r="A89" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>783</v>
@@ -33317,22 +33306,22 @@
         <v>767</v>
       </c>
       <c r="N89" s="7" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="O89" s="7" t="s">
         <v>784</v>
       </c>
       <c r="P89" s="7" t="s">
+        <v>1407</v>
+      </c>
+      <c r="Q89" s="7" t="s">
         <v>1408</v>
       </c>
-      <c r="Q89" s="7" t="s">
+      <c r="R89" s="7" t="s">
         <v>1409</v>
       </c>
-      <c r="R89" s="7" t="s">
+      <c r="S89" s="7" t="s">
         <v>1410</v>
-      </c>
-      <c r="S89" s="7" t="s">
-        <v>1411</v>
       </c>
       <c r="T89" s="7" t="s">
         <v>276</v>
@@ -33409,7 +33398,7 @@
     </row>
     <row r="90" spans="1:43" ht="105" hidden="1">
       <c r="A90" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>787</v>
@@ -33448,22 +33437,22 @@
         <v>767</v>
       </c>
       <c r="N90" s="7" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="O90" s="7" t="s">
         <v>788</v>
       </c>
       <c r="P90" s="7" t="s">
+        <v>1412</v>
+      </c>
+      <c r="Q90" s="7" t="s">
         <v>1413</v>
       </c>
-      <c r="Q90" s="7" t="s">
+      <c r="R90" s="7" t="s">
         <v>1414</v>
       </c>
-      <c r="R90" s="7" t="s">
+      <c r="S90" s="7" t="s">
         <v>1415</v>
-      </c>
-      <c r="S90" s="7" t="s">
-        <v>1416</v>
       </c>
       <c r="T90" s="7" t="s">
         <v>276</v>
@@ -33540,7 +33529,7 @@
     </row>
     <row r="91" spans="1:43" ht="105" hidden="1">
       <c r="A91" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>791</v>
@@ -33579,22 +33568,22 @@
         <v>767</v>
       </c>
       <c r="N91" s="7" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="O91" s="7" t="s">
         <v>792</v>
       </c>
       <c r="P91" s="7" t="s">
+        <v>1417</v>
+      </c>
+      <c r="Q91" s="7" t="s">
         <v>1418</v>
       </c>
-      <c r="Q91" s="7" t="s">
+      <c r="R91" s="7" t="s">
         <v>1419</v>
       </c>
-      <c r="R91" s="7" t="s">
+      <c r="S91" s="7" t="s">
         <v>1420</v>
-      </c>
-      <c r="S91" s="7" t="s">
-        <v>1421</v>
       </c>
       <c r="T91" s="7" t="s">
         <v>276</v>
@@ -33671,7 +33660,7 @@
     </row>
     <row r="92" spans="1:43" ht="90" hidden="1">
       <c r="A92" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>795</v>
@@ -33710,22 +33699,22 @@
         <v>767</v>
       </c>
       <c r="N92" s="7" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="O92" s="7" t="s">
         <v>796</v>
       </c>
       <c r="P92" s="7" t="s">
+        <v>1422</v>
+      </c>
+      <c r="Q92" s="7" t="s">
         <v>1423</v>
       </c>
-      <c r="Q92" s="7" t="s">
+      <c r="R92" s="7" t="s">
         <v>1424</v>
       </c>
-      <c r="R92" s="7" t="s">
+      <c r="S92" s="7" t="s">
         <v>1425</v>
-      </c>
-      <c r="S92" s="7" t="s">
-        <v>1426</v>
       </c>
       <c r="T92" s="7" t="s">
         <v>276</v>
@@ -33802,7 +33791,7 @@
     </row>
     <row r="93" spans="1:43" ht="147.94999999999999" hidden="1" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>799</v>
@@ -33841,22 +33830,22 @@
         <v>767</v>
       </c>
       <c r="N93" s="7" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O93" s="7" t="s">
         <v>800</v>
       </c>
       <c r="P93" s="7" t="s">
+        <v>1427</v>
+      </c>
+      <c r="Q93" s="7" t="s">
         <v>1428</v>
       </c>
-      <c r="Q93" s="7" t="s">
+      <c r="R93" s="7" t="s">
         <v>1429</v>
       </c>
-      <c r="R93" s="7" t="s">
+      <c r="S93" s="7" t="s">
         <v>1430</v>
-      </c>
-      <c r="S93" s="7" t="s">
-        <v>1431</v>
       </c>
       <c r="T93" s="7" t="s">
         <v>276</v>
@@ -33933,7 +33922,7 @@
     </row>
     <row r="94" spans="1:43" ht="75" hidden="1">
       <c r="A94" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>578</v>
@@ -34064,7 +34053,7 @@
     </row>
     <row r="95" spans="1:43" ht="315" hidden="1">
       <c r="A95" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>589</v>
@@ -34103,22 +34092,22 @@
         <v>591</v>
       </c>
       <c r="N95" s="7" t="s">
+        <v>1431</v>
+      </c>
+      <c r="O95" s="7" t="s">
         <v>1432</v>
       </c>
-      <c r="O95" s="7" t="s">
+      <c r="P95" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q95" s="7" t="s">
         <v>1433</v>
       </c>
-      <c r="P95" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q95" s="7" t="s">
+      <c r="R95" s="7" t="s">
         <v>1434</v>
       </c>
-      <c r="R95" s="7" t="s">
+      <c r="S95" s="7" t="s">
         <v>1435</v>
-      </c>
-      <c r="S95" s="7" t="s">
-        <v>1436</v>
       </c>
       <c r="T95" s="7" t="s">
         <v>276</v>
@@ -34187,15 +34176,15 @@
         <v>46</v>
       </c>
       <c r="AP95" s="7" t="s">
+        <v>1436</v>
+      </c>
+      <c r="AQ95" s="7" t="s">
         <v>1437</v>
-      </c>
-      <c r="AQ95" s="7" t="s">
-        <v>1438</v>
       </c>
     </row>
     <row r="96" spans="1:43" ht="60" hidden="1">
       <c r="A96" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>596</v>
@@ -34234,10 +34223,10 @@
         <v>46</v>
       </c>
       <c r="N96" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="O96" s="7" t="s">
         <v>1439</v>
-      </c>
-      <c r="O96" s="7" t="s">
-        <v>1440</v>
       </c>
       <c r="P96" s="7" t="s">
         <v>46</v>
@@ -34327,11 +34316,13 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:AQ96" xr:uid="{765A25C5-43E9-47DC-8427-7637ACFB5824}">
-    <filterColumn colId="0">
-      <colorFilter dxfId="0" cellColor="0"/>
+    <filterColumn colId="33">
+      <filters>
+        <filter val="Correction: 4/130 (3.08)"/>
+      </filters>
     </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AQ96">
-      <sortCondition sortBy="fontColor" ref="A1:A94" dxfId="1"/>
+      <sortCondition sortBy="fontColor" ref="A1:A94" dxfId="0"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>